<commit_message>
Data now comes from an xls
</commit_message>
<xml_diff>
--- a/supply.xlsx
+++ b/supply.xlsx
@@ -1,46 +1,145 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tulajdonos\Desktop\Tomasz diplomamunka\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuladonos\source\repos\Python\Other\Data\mavir_PSGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2D4433-F5AD-4EF9-8319-8890F635E866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39379C2-F319-4A82-A946-A927E68C622A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35472" yWindow="4068" windowWidth="5028" windowHeight="6972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IB" sheetId="1" r:id="rId1"/>
+    <sheet name="00" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">IB!$F$7</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>seller_id</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>volume</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>SZUMMA</t>
+  </si>
+  <si>
+    <t>afrr1</t>
+  </si>
+  <si>
+    <t>afrr2</t>
+  </si>
+  <si>
+    <t>afrr3</t>
+  </si>
+  <si>
+    <t>afrr4</t>
+  </si>
+  <si>
+    <t>afrr5</t>
+  </si>
+  <si>
+    <t>afrr6</t>
+  </si>
+  <si>
+    <t>afrr7</t>
+  </si>
+  <si>
+    <t>afrr8</t>
+  </si>
+  <si>
+    <t>mfrr1</t>
+  </si>
+  <si>
+    <t>mfrr2</t>
+  </si>
+  <si>
+    <t>mfrr3</t>
+  </si>
+  <si>
+    <t>mfrr4</t>
+  </si>
+  <si>
+    <t>mfrr5</t>
+  </si>
+  <si>
+    <t>mfrr6</t>
+  </si>
+  <si>
+    <t>mfrr7</t>
+  </si>
+  <si>
+    <t>mfrr8</t>
+  </si>
+  <si>
+    <t>mfrr9</t>
+  </si>
+  <si>
+    <t>mfrr10</t>
+  </si>
+  <si>
+    <t>mfrr11</t>
+  </si>
+  <si>
+    <t>mfrr12</t>
+  </si>
+  <si>
+    <t>mfrr13</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>afrrPiac</t>
+  </si>
+  <si>
+    <t>mfrrPiac</t>
+  </si>
+  <si>
+    <t>afrrVolume</t>
+  </si>
+  <si>
+    <t>afrrCost</t>
+  </si>
+  <si>
+    <t>mfrrVolume</t>
+  </si>
+  <si>
+    <t>mfrrCost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,13 +147,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,8 +197,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,59 +487,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>95</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>110</v>
-      </c>
-      <c r="C3">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>120</v>
-      </c>
-      <c r="C4">
-        <v>24</v>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" s="2">
+        <v>125.42700000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E7FEB5-E091-4120-8BD7-DFA6BAE6B632}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>145000</v>
+      </c>
+      <c r="G2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>122322</v>
+      </c>
+      <c r="D3">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>156999</v>
+      </c>
+      <c r="G3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>218978</v>
+      </c>
+      <c r="D4">
+        <v>164</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>157000</v>
+      </c>
+      <c r="G4">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>254652</v>
+      </c>
+      <c r="D5">
+        <v>197</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>159000</v>
+      </c>
+      <c r="G5">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>257130</v>
+      </c>
+      <c r="D6">
+        <v>232</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>160000</v>
+      </c>
+      <c r="G6">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>260000</v>
+      </c>
+      <c r="D7">
+        <v>237</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7">
+        <v>161997</v>
+      </c>
+      <c r="G7">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>260000</v>
+      </c>
+      <c r="D8">
+        <v>242</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>161998</v>
+      </c>
+      <c r="G8">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>260000</v>
+      </c>
+      <c r="D9">
+        <v>267</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9">
+        <v>161999</v>
+      </c>
+      <c r="G9">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="3"/>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>162000</v>
+      </c>
+      <c r="G10">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>162000</v>
+      </c>
+      <c r="G11">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>162000</v>
+      </c>
+      <c r="G12">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>162000</v>
+      </c>
+      <c r="G13">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14">
+        <v>162000</v>
+      </c>
+      <c r="G14">
+        <v>1269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated output values (added residual volume, cost by item)
</commit_message>
<xml_diff>
--- a/supply.xlsx
+++ b/supply.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuladonos\source\repos\Python\Other\Data\mavir_PSGA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0754C518-C852-4F7B-8448-40531ACAC2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AABFB08-296E-44F9-B6BC-1FA3155E03DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-96" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-96" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IB" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="139">
   <si>
     <t>SZUMMA</t>
   </si>
@@ -464,6 +464,9 @@
   <si>
     <t>mFRR es RR / mFRR and RR</t>
   </si>
+  <si>
+    <t>Negativ / Negative</t>
+  </si>
 </sst>
 </file>
 
@@ -653,7 +656,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$98</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -1281,7 +1284,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$98</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -1581,7 +1584,7 @@
             <c:numRef>
               <c:f>[1]IB!$L$2:$L$99</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="98"/>
                 <c:pt idx="0">
                   <c:v>125.42700000000001</c:v>
@@ -1906,7 +1909,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$98</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2206,7 +2209,7 @@
             <c:numRef>
               <c:f>[1]IB!$U$2:$U$99</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="98"/>
                 <c:pt idx="0">
                   <c:v>125.42700000000001</c:v>
@@ -2866,7 +2869,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$98</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -3166,7 +3169,7 @@
             <c:numRef>
               <c:f>[1]IB!$L$2:$L$98</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>125.42700000000001</c:v>
@@ -3482,7 +3485,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$97</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="96"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -3779,7 +3782,7 @@
             <c:numRef>
               <c:f>[1]IB!$Z$2:$Z$97</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="96"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4092,7 +4095,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$97</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="96"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -5013,7 +5016,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$98</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -5313,7 +5316,7 @@
             <c:numRef>
               <c:f>[1]IB!$L$2:$L$99</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="98"/>
                 <c:pt idx="0">
                   <c:v>125.42700000000001</c:v>
@@ -5988,7 +5991,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6050,7 +6053,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6220,7 +6223,7 @@
             <c:numRef>
               <c:f>[1]IB!$A$2:$A$98</c:f>
               <c:numCache>
-                <c:formatCode>h:mm</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="97"/>
                 <c:pt idx="0">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -6520,7 +6523,7 @@
             <c:numRef>
               <c:f>[1]IB!$L$2:$L$99</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="98"/>
                 <c:pt idx="0">
                   <c:v>125.42700000000001</c:v>
@@ -6969,7 +6972,7 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -9817,8 +9820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN160"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11119,14 +11122,14 @@
         <v>19</v>
       </c>
       <c r="D2" s="7">
-        <v>125.42700000000001</v>
+        <v>-125.42700000000001</v>
       </c>
       <c r="E2" s="7">
         <v>0</v>
       </c>
       <c r="F2" s="7">
         <f>D2+E2</f>
-        <v>125.42700000000001</v>
+        <v>-125.42700000000001</v>
       </c>
       <c r="G2" s="7">
         <v>115.89</v>
@@ -11145,14 +11148,14 @@
       </c>
       <c r="L2" s="2">
         <f>F2+K2</f>
-        <v>125.42700000000001</v>
+        <v>-125.42700000000001</v>
       </c>
       <c r="M2" s="8">
         <v>0</v>
       </c>
       <c r="N2">
         <f t="shared" ref="N2:N65" si="0">IF(L2&gt;0,L2,0)</f>
-        <v>125.42700000000001</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <f>IF(N2&lt;M2,1,0)</f>
@@ -11164,7 +11167,7 @@
       </c>
       <c r="Q2" s="2">
         <f>L2-M2</f>
-        <v>125.42700000000001</v>
+        <v>-125.42700000000001</v>
       </c>
       <c r="R2">
         <f t="shared" ref="R2:R65" si="1">IF(P2&gt;0,P2,0)</f>
@@ -11175,15 +11178,15 @@
       </c>
       <c r="T2" s="2">
         <f>L2-M2</f>
-        <v>125.42700000000001</v>
+        <v>-125.42700000000001</v>
       </c>
       <c r="U2" s="2">
         <f>N2-W2</f>
-        <v>125.42700000000001</v>
+        <v>0</v>
       </c>
       <c r="V2" s="2">
         <f>IF(U2&gt;0,U2,0)</f>
-        <v>125.42700000000001</v>
+        <v>0</v>
       </c>
       <c r="W2">
         <f>IF(N2-M2&gt;260,R2+N2-260,R2)</f>
@@ -11197,7 +11200,7 @@
       </c>
       <c r="Z2" s="2">
         <f>T2-U2</f>
-        <v>0</v>
+        <v>-125.42700000000001</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -11333,7 +11336,7 @@
       </c>
       <c r="M4" s="2">
         <f>IF(L2&gt;100,L2/3,0)</f>
-        <v>41.809000000000005</v>
+        <v>0</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
@@ -11345,34 +11348,34 @@
       </c>
       <c r="P4" s="2">
         <f t="shared" si="5"/>
-        <v>41.809000000000005</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="2">
         <f t="shared" si="6"/>
-        <v>35.205999999999996</v>
+        <v>77.015000000000001</v>
       </c>
       <c r="R4">
         <f t="shared" si="1"/>
-        <v>41.809000000000005</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <v>0</v>
       </c>
       <c r="T4" s="2">
         <f t="shared" si="7"/>
-        <v>35.205999999999996</v>
+        <v>77.015000000000001</v>
       </c>
       <c r="U4" s="2">
         <f t="shared" si="8"/>
-        <v>35.205999999999996</v>
+        <v>77.015000000000001</v>
       </c>
       <c r="V4" s="2">
         <f t="shared" si="9"/>
-        <v>35.205999999999996</v>
+        <v>77.015000000000001</v>
       </c>
       <c r="W4">
         <f t="shared" si="10"/>
-        <v>41.809000000000005</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -13626,7 +13629,7 @@
       </c>
       <c r="AC28" s="2">
         <f>SUM(N2:N98)*0.25</f>
-        <v>3496.1332499999994</v>
+        <v>3464.7764999999995</v>
       </c>
       <c r="AD28" t="s">
         <v>49</v>
@@ -13636,7 +13639,7 @@
       </c>
       <c r="AG28">
         <f>SUM(N2:N98)*0.25</f>
-        <v>3496.1332499999994</v>
+        <v>3464.7764999999995</v>
       </c>
       <c r="AH28" t="s">
         <v>49</v>
@@ -13758,7 +13761,7 @@
       </c>
       <c r="AG29">
         <f>SUM(R2:R99)*0.25</f>
-        <v>967.16016666666678</v>
+        <v>956.70791666666673</v>
       </c>
       <c r="AH29" t="s">
         <v>49</v>
@@ -13876,7 +13879,7 @@
       </c>
       <c r="AC30" s="2">
         <f>AC28-AC29</f>
-        <v>2622.8829999999994</v>
+        <v>2591.5262499999994</v>
       </c>
       <c r="AD30" t="s">
         <v>49</v>
@@ -13886,7 +13889,7 @@
       </c>
       <c r="AG30">
         <f>SUM(N2:N99)*0.25-AG29</f>
-        <v>2528.9730833333324</v>
+        <v>2508.0685833333328</v>
       </c>
       <c r="AH30" t="s">
         <v>49</v>
@@ -17698,7 +17701,7 @@
         <v>133.869</v>
       </c>
       <c r="M70" s="2">
-        <f t="shared" ref="M70:M101" si="27">IF(L68&gt;100,L68/3,0)</f>
+        <f t="shared" ref="M70:M99" si="27">IF(L68&gt;100,L68/3,0)</f>
         <v>42.517666666666663</v>
       </c>
       <c r="N70">
@@ -21054,16 +21057,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E7FEB5-E091-4120-8BD7-DFA6BAE6B632}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
@@ -21282,7 +21285,7 @@
         <v>260000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>44525</v>
       </c>
@@ -21579,6 +21582,546 @@
       </c>
       <c r="G22">
         <v>162000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>-499000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24">
+        <v>63</v>
+      </c>
+      <c r="F24">
+        <v>-308244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+      <c r="C25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25">
+        <v>19</v>
+      </c>
+      <c r="F25">
+        <v>-279499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <v>-121000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+      <c r="F27">
+        <v>-120000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>-75000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29">
+        <v>38</v>
+      </c>
+      <c r="F29">
+        <v>-34999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>-33000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>-25000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32">
+        <v>156</v>
+      </c>
+      <c r="F32">
+        <v>-5554</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33">
+        <v>70</v>
+      </c>
+      <c r="F33">
+        <v>-3321</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" t="s">
+        <v>138</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>-550</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C36" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>-100000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>-53000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>-53000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40">
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <v>-53000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41">
+        <v>13</v>
+      </c>
+      <c r="F41">
+        <v>-53000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
+        <v>137</v>
+      </c>
+      <c r="D42" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42">
+        <v>25</v>
+      </c>
+      <c r="F42">
+        <v>-53000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>-41900</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B44" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" t="s">
+        <v>138</v>
+      </c>
+      <c r="E44">
+        <v>6</v>
+      </c>
+      <c r="F44">
+        <v>-41900</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B45" t="s">
+        <v>134</v>
+      </c>
+      <c r="C45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" t="s">
+        <v>138</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>-41000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>-41000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B47" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" t="s">
+        <v>138</v>
+      </c>
+      <c r="E47">
+        <v>25</v>
+      </c>
+      <c r="F47">
+        <v>-41000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" t="s">
+        <v>137</v>
+      </c>
+      <c r="D48" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>44197</v>
+      </c>
+      <c r="B49" t="s">
+        <v>134</v>
+      </c>
+      <c r="C49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" t="s">
+        <v>138</v>
+      </c>
+      <c r="E49">
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>